<commit_message>
🧹 Cleaned FRs - Marked some FRs than need to be deleted - Marked each FR's type (user, owner, renter, admin, or system)
</commit_message>
<xml_diff>
--- a/Requirements/Requirments.xlsx
+++ b/Requirements/Requirments.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED273BB-907A-4617-9748-8B08546FF414}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D2F36-44DA-4710-80D1-248C7B4FA2F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FRs" sheetId="1" r:id="rId1"/>
+    <sheet name="FRs Cleaning" sheetId="2" r:id="rId2"/>
+    <sheet name="NFRs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="153">
   <si>
     <t>id</t>
   </si>
@@ -517,6 +519,261 @@
   <si>
     <t>Created 9/3/21</t>
   </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Types</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ser
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">wner
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">enter
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">dmin
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ystem</t>
+    </r>
+  </si>
+  <si>
+    <t>U/A/S?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Color codes:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF4F4F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+⬛ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Delete
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>⬛</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Caution</t>
+    </r>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>U/S?</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>O/S?</t>
+  </si>
+  <si>
+    <t>The system must allow the owner to edit and delete their posts</t>
+  </si>
+  <si>
+    <t>O/U/S?</t>
+  </si>
+  <si>
+    <t>O/U?</t>
+  </si>
+  <si>
+    <t>The system must allow the owner to view tool-requests sent to their posts</t>
+  </si>
+  <si>
+    <t>The system must allow the owner to accept a tool-request</t>
+  </si>
+  <si>
+    <t>R/U?</t>
+  </si>
+  <si>
+    <t>Created 5/3/21
+Edited 9/3/21</t>
+  </si>
+  <si>
+    <t>The system must allow the renter to send a tool-request to a post.</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>The system must allow the renter to edit or remove his/her tool-request</t>
+  </si>
+  <si>
+    <t>S/U/A?</t>
+  </si>
+  <si>
+    <t>Created 9/3/21
+Edited 9/3/21</t>
+  </si>
+  <si>
+    <t>The system must allow the owner to calim the tool is damaged.</t>
+  </si>
 </sst>
 </file>
 
@@ -525,7 +782,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\F\R0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,8 +798,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF4F4F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -552,6 +846,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4F4F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -600,12 +906,38 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF4F4F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -880,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +1282,6 @@
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -974,7 +1305,6 @@
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A48" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -995,7 +1325,6 @@
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1019,7 +1348,6 @@
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1040,7 +1368,6 @@
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1061,7 +1388,6 @@
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1079,7 +1405,6 @@
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1097,7 +1422,6 @@
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1118,7 +1442,6 @@
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1139,7 +1462,6 @@
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1163,7 +1485,6 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1178,7 +1499,6 @@
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1196,7 +1516,6 @@
     </row>
     <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1214,7 +1533,6 @@
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1235,7 +1553,6 @@
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1259,7 +1576,6 @@
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1277,7 +1593,6 @@
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1301,7 +1616,6 @@
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1322,7 +1636,6 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1340,7 +1653,6 @@
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1358,7 +1670,6 @@
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1376,7 +1687,6 @@
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1394,7 +1704,6 @@
     </row>
     <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1412,7 +1721,6 @@
     </row>
     <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1430,7 +1738,6 @@
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1448,7 +1755,6 @@
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1466,7 +1772,6 @@
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1484,7 +1789,6 @@
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1502,7 +1806,6 @@
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1520,7 +1823,6 @@
     </row>
     <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1538,7 +1840,6 @@
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1556,7 +1857,6 @@
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1574,7 +1874,6 @@
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1592,7 +1891,6 @@
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <f>A35+1</f>
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1610,7 +1908,6 @@
     </row>
     <row r="37" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <f>A36+1</f>
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1628,7 +1925,6 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1646,7 +1942,6 @@
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <f>A38+1</f>
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1661,7 +1956,6 @@
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <f>A39+1</f>
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1676,7 +1970,6 @@
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <f>A40+1</f>
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1694,7 +1987,6 @@
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1712,7 +2004,6 @@
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1727,7 +2018,6 @@
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1738,34 +2028,1014 @@
       </c>
       <c r="H44" s="1" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
-        <f t="shared" si="0"/>
-        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2D3E01-40A2-497A-AC28-649813C7548F}">
+  <dimension ref="A1:M51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="15.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>18</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>21</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>22</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>27</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>29</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>31</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>32</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>33</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>34</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>35</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>36</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D7737-055D-47E1-B3C5-9E700893BA8A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
📝 Added an FR for search
</commit_message>
<xml_diff>
--- a/Requirements/Requirments.xlsx
+++ b/Requirements/Requirments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D2F36-44DA-4710-80D1-248C7B4FA2F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C86C823-BBA8-49D6-A1D1-5157CE57B46B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="157">
   <si>
     <t>id</t>
   </si>
@@ -774,6 +774,19 @@
   <si>
     <t>The system must allow the owner to calim the tool is damaged.</t>
   </si>
+  <si>
+    <t>A search bar will be displayed.
+When the user searches, a list of tool-posts that match the search query will be displayed</t>
+  </si>
+  <si>
+    <t>The system must allow the user to search for a tool-post.</t>
+  </si>
+  <si>
+    <t>FR44</t>
+  </si>
+  <si>
+    <t>FR37</t>
+  </si>
 </sst>
 </file>
 
@@ -889,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -920,6 +933,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1212,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,6 +2046,20 @@
         <v>128</v>
       </c>
     </row>
+    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2038,10 +2068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2D3E01-40A2-497A-AC28-649813C7548F}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,10 +2145,10 @@
       <c r="I2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="13" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2147,8 +2177,8 @@
       <c r="I3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -2981,39 +3011,23 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
-        <v>43</v>
+    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3030,7 +3044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D7737-055D-47E1-B3C5-9E700893BA8A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
🧹 Seperated delted FRs from the others (in the cleaned sheet)
</commit_message>
<xml_diff>
--- a/Requirements/Requirments.xlsx
+++ b/Requirements/Requirments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C86C823-BBA8-49D6-A1D1-5157CE57B46B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F174B6-2112-4B63-B975-DE097553B5E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="158">
   <si>
     <t>id</t>
   </si>
@@ -787,6 +787,9 @@
   <si>
     <t>FR37</t>
   </si>
+  <si>
+    <t>Deleted FRs</t>
+  </si>
 </sst>
 </file>
 
@@ -795,7 +798,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\F\R0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,8 +851,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -874,8 +892,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -898,11 +921,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -919,17 +980,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -943,8 +995,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2068,10 +2136,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2D3E01-40A2-497A-AC28-649813C7548F}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,7 +2184,7 @@
       <c r="I1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="2" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2145,10 +2213,10 @@
       <c r="I2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="10" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2177,8 +2245,8 @@
       <c r="I3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="13"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -2230,21 +2298,22 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6" t="s">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -2253,19 +2322,16 @@
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
@@ -2274,587 +2340,585 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="J11" s="10"/>
+        <v>128</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="6" t="s">
-        <v>21</v>
+      <c r="I15" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>15</v>
-      </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>16</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>17</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>18</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>145</v>
+      <c r="I26" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>25</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>128</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>28</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>128</v>
@@ -2863,177 +2927,187 @@
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>29</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>128</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>30</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I38" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>31</v>
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>115</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
       <c r="H39" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I39" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>32</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>33</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="I39" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G48" s="14"/>
+      <c r="H48" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="D49" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
-        <v>36</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>131</v>
+      <c r="E49" s="13"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G50" s="14"/>
+      <c r="H50" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G51" s="14"/>
+      <c r="H51" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B53" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="13"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B54" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="13"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="15" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="B47:H47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
✔ Finished the FRs table
</commit_message>
<xml_diff>
--- a/Requirements/Requirments.xlsx
+++ b/Requirements/Requirments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F174B6-2112-4B63-B975-DE097553B5E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D61BA7-20DD-41E5-972C-6E8D2393A9DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="206">
   <si>
     <t>id</t>
   </si>
@@ -665,9 +665,6 @@
     </r>
   </si>
   <si>
-    <t>U/A/S?</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -725,31 +722,16 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>U/S?</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
-    <t>O/S?</t>
-  </si>
-  <si>
     <t>The system must allow the owner to edit and delete their posts</t>
   </si>
   <si>
-    <t>O/U/S?</t>
-  </si>
-  <si>
-    <t>O/U?</t>
-  </si>
-  <si>
     <t>The system must allow the owner to view tool-requests sent to their posts</t>
   </si>
   <si>
     <t>The system must allow the owner to accept a tool-request</t>
-  </si>
-  <si>
-    <t>R/U?</t>
   </si>
   <si>
     <t>Created 5/3/21
@@ -765,9 +747,6 @@
     <t>The system must allow the renter to edit or remove his/her tool-request</t>
   </si>
   <si>
-    <t>S/U/A?</t>
-  </si>
-  <si>
     <t>Created 9/3/21
 Edited 9/3/21</t>
   </si>
@@ -789,6 +768,171 @@
   </si>
   <si>
     <t>Deleted FRs</t>
+  </si>
+  <si>
+    <t>UC1, UC4, UC5, UC8</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>FR2</t>
+  </si>
+  <si>
+    <t>UC4, UC7</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>To add an easier and quicker method of singing in</t>
+  </si>
+  <si>
+    <t>To be able to identify the user and allow the user to access the system functionalities</t>
+  </si>
+  <si>
+    <t>To prevent unauthorized access to a user's account</t>
+  </si>
+  <si>
+    <t>To prevent a banned user from accessing the system</t>
+  </si>
+  <si>
+    <t>To prevent the banned user from ever accessing the system's functionalities</t>
+  </si>
+  <si>
+    <t>To prevent fake cards</t>
+  </si>
+  <si>
+    <t>To rent their tools, and for renters to send them tool-requests</t>
+  </si>
+  <si>
+    <t>The system must be able to determine if a user is authorized to create a new post.</t>
+  </si>
+  <si>
+    <t>To prevent unauthorized accounts from creating posts and filling the database</t>
+  </si>
+  <si>
+    <t>To prevent the posts from being edited by unauthorized user</t>
+  </si>
+  <si>
+    <t>To alert the user of any important information</t>
+  </si>
+  <si>
+    <t>For the owner to accept it and rent the tool to the renter</t>
+  </si>
+  <si>
+    <t>To start renting the tool to the renter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To either rent the tool to the renter or refuse his request and remove it from the tool-requests list </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the owner and renter to communicate </t>
+  </si>
+  <si>
+    <t>To prevent unauthorized access to a tool-request</t>
+  </si>
+  <si>
+    <t>To allow the renter to change his tool-request details or delete the request entirely</t>
+  </si>
+  <si>
+    <t>To allow them to rate each other</t>
+  </si>
+  <si>
+    <t>To prevent an unauthorized user from deleting a review</t>
+  </si>
+  <si>
+    <t>To express his/her expirence with the other user</t>
+  </si>
+  <si>
+    <t>To remove the review from the user's profile</t>
+  </si>
+  <si>
+    <t>to upload pictures and videos of a tool</t>
+  </si>
+  <si>
+    <t>To take pictures and videos of a tool</t>
+  </si>
+  <si>
+    <t>To send money between users and from the system to the users</t>
+  </si>
+  <si>
+    <t>To inform the user of specific information</t>
+  </si>
+  <si>
+    <t>So the admin can settle and fix the problem</t>
+  </si>
+  <si>
+    <t>So the admin can review the problem and arrive to a decission</t>
+  </si>
+  <si>
+    <t>To prevent the renter from damaging the tool without paying for it</t>
+  </si>
+  <si>
+    <t>To send the appropiate amount of money to each the owner and renter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To upload any official documents </t>
+  </si>
+  <si>
+    <t>So the owner and renter can agree on a middle ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To find a tool-post of a specific tool so the renter can send a tool-request </t>
+  </si>
+  <si>
+    <t>FR7, FR2</t>
+  </si>
+  <si>
+    <t>FR1, FR2, FR11</t>
+  </si>
+  <si>
+    <t>FR2, FR11, FR13</t>
+  </si>
+  <si>
+    <t>FR2, FR11, FR21</t>
+  </si>
+  <si>
+    <t>FR2, FR11, FR16, FR17, FR21</t>
+  </si>
+  <si>
+    <t>FR2, FR11, FR16, FR21</t>
+  </si>
+  <si>
+    <t>FR2, FR4</t>
+  </si>
+  <si>
+    <t>FR2, FR11, FR20</t>
+  </si>
+  <si>
+    <t>FR1, FR2, FR12</t>
+  </si>
+  <si>
+    <t>FR2, FR20, FR21</t>
+  </si>
+  <si>
+    <t>FR1, FR2, FR23</t>
+  </si>
+  <si>
+    <t>FR2, FR24</t>
+  </si>
+  <si>
+    <t>FR2, FR24, FR25</t>
+  </si>
+  <si>
+    <t>FR27</t>
+  </si>
+  <si>
+    <t>FR4</t>
   </si>
 </sst>
 </file>
@@ -963,7 +1107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -990,12 +1134,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1009,6 +1147,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1296,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:H47"/>
+    <sheetView topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,19 +2266,170 @@
     </row>
     <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>128</v>
       </c>
     </row>
+    <row r="50" spans="3:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C50" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+    </row>
+    <row r="51" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C51" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="11"/>
+      <c r="G51" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C52" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C53" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" s="11"/>
+      <c r="G53" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C54" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C55" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="C56" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="11"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="C57" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C50:J50"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2136,10 +2437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2D3E01-40A2-497A-AC28-649813C7548F}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,13 +2451,14 @@
     <col min="4" max="4" width="31.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="29.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="11.85546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="15.7109375" style="1"/>
+    <col min="7" max="7" width="10.140625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="9" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="11.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="15.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2176,19 +2478,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2207,20 +2512,23 @@
       <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="N2" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2234,21 +2542,24 @@
         <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="M3" s="16"/>
+      <c r="N3" s="17"/>
+    </row>
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2261,17 +2572,23 @@
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="F4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2288,16 +2605,19 @@
         <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2310,17 +2630,23 @@
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="F6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2333,14 +2659,23 @@
       <c r="D7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2353,17 +2688,23 @@
       <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="F8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2376,23 +2717,29 @@
       <c r="D9" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="J9" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>125</v>
@@ -2404,33 +2751,48 @@
         <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2443,14 +2805,23 @@
       <c r="D12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="J12" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2458,19 +2829,28 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="J13" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2478,7 +2858,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>49</v>
@@ -2486,17 +2866,20 @@
       <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="F14" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2509,14 +2892,23 @@
       <c r="D15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J15" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2529,14 +2921,23 @@
       <c r="D16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2549,14 +2950,23 @@
       <c r="D17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J17" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2564,19 +2974,28 @@
         <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2584,19 +3003,28 @@
         <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J19" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2609,14 +3037,23 @@
       <c r="D20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="E20" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2629,14 +3066,23 @@
       <c r="D21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="E21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J21" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2644,19 +3090,28 @@
         <v>68</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>146</v>
+      <c r="E22" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2664,19 +3119,28 @@
         <v>76</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>146</v>
+      <c r="E23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2689,14 +3153,23 @@
       <c r="D24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="E24" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2709,14 +3182,23 @@
       <c r="D25" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -2729,14 +3211,23 @@
       <c r="D26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="E26" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -2749,14 +3240,23 @@
       <c r="D27" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="E27" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -2769,14 +3269,23 @@
       <c r="D28" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2789,14 +3298,23 @@
       <c r="D29" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="E29" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -2809,14 +3327,23 @@
       <c r="D30" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="E30" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -2829,48 +3356,81 @@
       <c r="D31" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
+      <c r="B32" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="E32" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I32" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J32" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
+      <c r="B33" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="E33" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -2878,19 +3438,28 @@
         <v>111</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>151</v>
+      <c r="E34" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -2903,211 +3472,114 @@
       <c r="D35" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J35" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
+      <c r="B36" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="C36" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="E36" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="C37" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="E37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" s="1" t="s">
+    <row r="38" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="1" t="s">
+      <c r="H38" s="8"/>
+      <c r="I38" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-    </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="13"/>
-      <c r="F48" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B50" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E50" s="13"/>
-      <c r="F50" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G50" s="14"/>
-      <c r="H50" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B51" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G51" s="14"/>
-      <c r="H51" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E53" s="13"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B54" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E54" s="13"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="L2:L3"/>
+  <mergeCells count="2">
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3119,7 +3591,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>